<commit_message>
changed graphics, corrected conclusions and the presentation index
</commit_message>
<xml_diff>
--- a/written/presentation/excels/MontecarloPhase.xlsx
+++ b/written/presentation/excels/MontecarloPhase.xlsx
@@ -178,214 +178,214 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="70"/>
                   <c:pt idx="0">
-                    <c:v>104.838671306191</c:v>
+                    <c:v>85.051000068270596</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>102.29111208984</c:v>
+                    <c:v>83.545042422626196</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>102.05013617433799</c:v>
+                    <c:v>82.776149638236106</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>100.842466787677</c:v>
+                    <c:v>82.624740075180995</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>100.565405933363</c:v>
+                    <c:v>86.304328143395395</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>99.425776980452397</c:v>
+                    <c:v>81.237954199280907</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>99.391387237600796</c:v>
+                    <c:v>82.225810410563099</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>98.497121431295895</c:v>
+                    <c:v>85.792131824098703</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>99.495419745672095</c:v>
+                    <c:v>86.506323016713594</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>100.16072469089499</c:v>
+                    <c:v>81.8971269724519</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>112.80707952471499</c:v>
+                    <c:v>115.597280052011</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>100.671111382531</c:v>
+                    <c:v>84.051944619351104</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>101.013391876486</c:v>
+                    <c:v>82.548378261890406</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>97.943175694066497</c:v>
+                    <c:v>83.400048488353505</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>98.3888271217143</c:v>
+                    <c:v>83.124704459000995</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>99.069619310494801</c:v>
+                    <c:v>84.894276343970702</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>96.927833873323607</c:v>
+                    <c:v>83.485936866112894</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>102.26012677997301</c:v>
+                    <c:v>85.363057623032105</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>97.490487164652393</c:v>
+                    <c:v>86.086235312413294</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>96.201514272612798</c:v>
+                    <c:v>85.502794142896605</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>101.99076581904301</c:v>
+                    <c:v>84.815465449479007</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>99.709325381999804</c:v>
+                    <c:v>83.756172733130398</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>102.869996536557</c:v>
+                    <c:v>84.629320475430802</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>102.713694188217</c:v>
+                    <c:v>84.291044484866006</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>97.4714040165113</c:v>
+                    <c:v>85.284252007254494</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>100.811182367423</c:v>
+                    <c:v>85.264297957082505</c:v>
                   </c:pt>
                   <c:pt idx="26">
-                    <c:v>100.027118856602</c:v>
+                    <c:v>83.069413889312102</c:v>
                   </c:pt>
                   <c:pt idx="27">
-                    <c:v>96.221111702426498</c:v>
+                    <c:v>85.509566945733297</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>100.318111756931</c:v>
+                    <c:v>85.512167142847503</c:v>
                   </c:pt>
                   <c:pt idx="29">
-                    <c:v>102.846837755156</c:v>
+                    <c:v>83.493105784984493</c:v>
                   </c:pt>
                   <c:pt idx="30">
-                    <c:v>98.400686020703702</c:v>
+                    <c:v>82.731672923523305</c:v>
                   </c:pt>
                   <c:pt idx="31">
-                    <c:v>99.515041390427598</c:v>
+                    <c:v>83.026084948991596</c:v>
                   </c:pt>
                   <c:pt idx="32">
-                    <c:v>98.875548476422907</c:v>
+                    <c:v>83.860137388589806</c:v>
                   </c:pt>
                   <c:pt idx="33">
-                    <c:v>102.39863625739601</c:v>
+                    <c:v>83.572044489308297</c:v>
                   </c:pt>
                   <c:pt idx="34">
-                    <c:v>98.733556395947303</c:v>
+                    <c:v>82.132281142149594</c:v>
                   </c:pt>
                   <c:pt idx="35">
-                    <c:v>97.791815712052994</c:v>
+                    <c:v>81.710724849113404</c:v>
                   </c:pt>
                   <c:pt idx="36">
-                    <c:v>99.676727093416304</c:v>
+                    <c:v>83.961438137922698</c:v>
                   </c:pt>
                   <c:pt idx="37">
-                    <c:v>98.643907501151205</c:v>
+                    <c:v>83.666107009785705</c:v>
                   </c:pt>
                   <c:pt idx="38">
-                    <c:v>102.43705941507601</c:v>
+                    <c:v>84.060798014025195</c:v>
                   </c:pt>
                   <c:pt idx="39">
-                    <c:v>97.725078826283905</c:v>
+                    <c:v>84.1053053152486</c:v>
                   </c:pt>
                   <c:pt idx="40">
-                    <c:v>99.652085349332296</c:v>
+                    <c:v>82.796274596050793</c:v>
                   </c:pt>
                   <c:pt idx="41">
-                    <c:v>99.902023924803302</c:v>
+                    <c:v>84.697772456638504</c:v>
                   </c:pt>
                   <c:pt idx="42">
-                    <c:v>96.771219936602094</c:v>
+                    <c:v>86.316181523646193</c:v>
                   </c:pt>
                   <c:pt idx="43">
-                    <c:v>114.541229089569</c:v>
+                    <c:v>113.273392492122</c:v>
                   </c:pt>
                   <c:pt idx="44">
-                    <c:v>99.074667099206906</c:v>
+                    <c:v>83.902023055044296</c:v>
                   </c:pt>
                   <c:pt idx="45">
-                    <c:v>98.553402029472295</c:v>
+                    <c:v>83.025747999464301</c:v>
                   </c:pt>
                   <c:pt idx="46">
-                    <c:v>97.622958729129806</c:v>
+                    <c:v>84.625005834080696</c:v>
                   </c:pt>
                   <c:pt idx="47">
-                    <c:v>99.467916907682294</c:v>
+                    <c:v>83.613976875084802</c:v>
                   </c:pt>
                   <c:pt idx="48">
-                    <c:v>98.434588836287006</c:v>
+                    <c:v>83.919351687935702</c:v>
                   </c:pt>
                   <c:pt idx="49">
-                    <c:v>101.112711512328</c:v>
+                    <c:v>85.020512128505999</c:v>
                   </c:pt>
                   <c:pt idx="50">
-                    <c:v>97.210044501225099</c:v>
+                    <c:v>84.387631605532505</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>99.496456623990298</c:v>
+                    <c:v>84.830913021837205</c:v>
                   </c:pt>
                   <c:pt idx="52">
-                    <c:v>99.6832894932638</c:v>
+                    <c:v>83.152455901366395</c:v>
                   </c:pt>
                   <c:pt idx="53">
-                    <c:v>101.476796027885</c:v>
+                    <c:v>84.476678208048895</c:v>
                   </c:pt>
                   <c:pt idx="54">
-                    <c:v>96.734064379037903</c:v>
+                    <c:v>87.113980806857697</c:v>
                   </c:pt>
                   <c:pt idx="55">
-                    <c:v>110.92038157853101</c:v>
+                    <c:v>113.394608277892</c:v>
                   </c:pt>
                   <c:pt idx="56">
-                    <c:v>101.873964572437</c:v>
+                    <c:v>84.324308433550698</c:v>
                   </c:pt>
                   <c:pt idx="57">
-                    <c:v>97.901813315181002</c:v>
+                    <c:v>84.938488916882406</c:v>
                   </c:pt>
                   <c:pt idx="58">
-                    <c:v>100.78946705880399</c:v>
+                    <c:v>83.731193285324593</c:v>
                   </c:pt>
                   <c:pt idx="59">
-                    <c:v>99.689668061715196</c:v>
+                    <c:v>83.221774284760798</c:v>
                   </c:pt>
                   <c:pt idx="60">
-                    <c:v>103.516594224153</c:v>
+                    <c:v>84.203290393247201</c:v>
                   </c:pt>
                   <c:pt idx="61">
-                    <c:v>95.759293716147297</c:v>
+                    <c:v>82.057665337044995</c:v>
                   </c:pt>
                   <c:pt idx="62">
-                    <c:v>100.387918098631</c:v>
+                    <c:v>82.665659158335401</c:v>
                   </c:pt>
                   <c:pt idx="63">
-                    <c:v>97.261723203409204</c:v>
+                    <c:v>81.766857573413603</c:v>
                   </c:pt>
                   <c:pt idx="64">
-                    <c:v>101.22072392242499</c:v>
+                    <c:v>88.249724968299603</c:v>
                   </c:pt>
                   <c:pt idx="65">
-                    <c:v>102.002803578315</c:v>
+                    <c:v>84.647924673243196</c:v>
                   </c:pt>
                   <c:pt idx="66">
-                    <c:v>100.892933790336</c:v>
+                    <c:v>87.910430936452698</c:v>
                   </c:pt>
                   <c:pt idx="67">
-                    <c:v>99.381532000379806</c:v>
+                    <c:v>85.906475062918304</c:v>
                   </c:pt>
                   <c:pt idx="68">
-                    <c:v>103.943241126937</c:v>
+                    <c:v>84.768727843478203</c:v>
                   </c:pt>
                   <c:pt idx="69">
-                    <c:v>99.2999859174204</c:v>
+                    <c:v>85.191755519779093</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -397,214 +397,214 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="70"/>
                   <c:pt idx="0">
-                    <c:v>104.838671306191</c:v>
+                    <c:v>85.051000068270596</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>102.29111208984</c:v>
+                    <c:v>83.545042422626196</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>102.05013617433799</c:v>
+                    <c:v>82.776149638236106</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>100.842466787677</c:v>
+                    <c:v>82.624740075180995</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>100.565405933363</c:v>
+                    <c:v>86.304328143395395</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>99.425776980452397</c:v>
+                    <c:v>81.237954199280907</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>99.391387237600796</c:v>
+                    <c:v>82.225810410563099</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>98.497121431295895</c:v>
+                    <c:v>85.792131824098703</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>99.495419745672095</c:v>
+                    <c:v>86.506323016713594</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>100.16072469089499</c:v>
+                    <c:v>81.8971269724519</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>112.80707952471499</c:v>
+                    <c:v>115.597280052011</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>100.671111382531</c:v>
+                    <c:v>84.051944619351104</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>101.013391876486</c:v>
+                    <c:v>82.548378261890406</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>97.943175694066497</c:v>
+                    <c:v>83.400048488353505</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>98.3888271217143</c:v>
+                    <c:v>83.124704459000995</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>99.069619310494801</c:v>
+                    <c:v>84.894276343970702</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>96.927833873323607</c:v>
+                    <c:v>83.485936866112894</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>102.26012677997301</c:v>
+                    <c:v>85.363057623032105</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>97.490487164652393</c:v>
+                    <c:v>86.086235312413294</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>96.201514272612798</c:v>
+                    <c:v>85.502794142896605</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>101.99076581904301</c:v>
+                    <c:v>84.815465449479007</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>99.709325381999804</c:v>
+                    <c:v>83.756172733130398</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>102.869996536557</c:v>
+                    <c:v>84.629320475430802</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>102.713694188217</c:v>
+                    <c:v>84.291044484866006</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>97.4714040165113</c:v>
+                    <c:v>85.284252007254494</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>100.811182367423</c:v>
+                    <c:v>85.264297957082505</c:v>
                   </c:pt>
                   <c:pt idx="26">
-                    <c:v>100.027118856602</c:v>
+                    <c:v>83.069413889312102</c:v>
                   </c:pt>
                   <c:pt idx="27">
-                    <c:v>96.221111702426498</c:v>
+                    <c:v>85.509566945733297</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>100.318111756931</c:v>
+                    <c:v>85.512167142847503</c:v>
                   </c:pt>
                   <c:pt idx="29">
-                    <c:v>102.846837755156</c:v>
+                    <c:v>83.493105784984493</c:v>
                   </c:pt>
                   <c:pt idx="30">
-                    <c:v>98.400686020703702</c:v>
+                    <c:v>82.731672923523305</c:v>
                   </c:pt>
                   <c:pt idx="31">
-                    <c:v>99.515041390427598</c:v>
+                    <c:v>83.026084948991596</c:v>
                   </c:pt>
                   <c:pt idx="32">
-                    <c:v>98.875548476422907</c:v>
+                    <c:v>83.860137388589806</c:v>
                   </c:pt>
                   <c:pt idx="33">
-                    <c:v>102.39863625739601</c:v>
+                    <c:v>83.572044489308297</c:v>
                   </c:pt>
                   <c:pt idx="34">
-                    <c:v>98.733556395947303</c:v>
+                    <c:v>82.132281142149594</c:v>
                   </c:pt>
                   <c:pt idx="35">
-                    <c:v>97.791815712052994</c:v>
+                    <c:v>81.710724849113404</c:v>
                   </c:pt>
                   <c:pt idx="36">
-                    <c:v>99.676727093416304</c:v>
+                    <c:v>83.961438137922698</c:v>
                   </c:pt>
                   <c:pt idx="37">
-                    <c:v>98.643907501151205</c:v>
+                    <c:v>83.666107009785705</c:v>
                   </c:pt>
                   <c:pt idx="38">
-                    <c:v>102.43705941507601</c:v>
+                    <c:v>84.060798014025195</c:v>
                   </c:pt>
                   <c:pt idx="39">
-                    <c:v>97.725078826283905</c:v>
+                    <c:v>84.1053053152486</c:v>
                   </c:pt>
                   <c:pt idx="40">
-                    <c:v>99.652085349332296</c:v>
+                    <c:v>82.796274596050793</c:v>
                   </c:pt>
                   <c:pt idx="41">
-                    <c:v>99.902023924803302</c:v>
+                    <c:v>84.697772456638504</c:v>
                   </c:pt>
                   <c:pt idx="42">
-                    <c:v>96.771219936602094</c:v>
+                    <c:v>86.316181523646193</c:v>
                   </c:pt>
                   <c:pt idx="43">
-                    <c:v>114.541229089569</c:v>
+                    <c:v>113.273392492122</c:v>
                   </c:pt>
                   <c:pt idx="44">
-                    <c:v>99.074667099206906</c:v>
+                    <c:v>83.902023055044296</c:v>
                   </c:pt>
                   <c:pt idx="45">
-                    <c:v>98.553402029472295</c:v>
+                    <c:v>83.025747999464301</c:v>
                   </c:pt>
                   <c:pt idx="46">
-                    <c:v>97.622958729129806</c:v>
+                    <c:v>84.625005834080696</c:v>
                   </c:pt>
                   <c:pt idx="47">
-                    <c:v>99.467916907682294</c:v>
+                    <c:v>83.613976875084802</c:v>
                   </c:pt>
                   <c:pt idx="48">
-                    <c:v>98.434588836287006</c:v>
+                    <c:v>83.919351687935702</c:v>
                   </c:pt>
                   <c:pt idx="49">
-                    <c:v>101.112711512328</c:v>
+                    <c:v>85.020512128505999</c:v>
                   </c:pt>
                   <c:pt idx="50">
-                    <c:v>97.210044501225099</c:v>
+                    <c:v>84.387631605532505</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>99.496456623990298</c:v>
+                    <c:v>84.830913021837205</c:v>
                   </c:pt>
                   <c:pt idx="52">
-                    <c:v>99.6832894932638</c:v>
+                    <c:v>83.152455901366395</c:v>
                   </c:pt>
                   <c:pt idx="53">
-                    <c:v>101.476796027885</c:v>
+                    <c:v>84.476678208048895</c:v>
                   </c:pt>
                   <c:pt idx="54">
-                    <c:v>96.734064379037903</c:v>
+                    <c:v>87.113980806857697</c:v>
                   </c:pt>
                   <c:pt idx="55">
-                    <c:v>110.92038157853101</c:v>
+                    <c:v>113.394608277892</c:v>
                   </c:pt>
                   <c:pt idx="56">
-                    <c:v>101.873964572437</c:v>
+                    <c:v>84.324308433550698</c:v>
                   </c:pt>
                   <c:pt idx="57">
-                    <c:v>97.901813315181002</c:v>
+                    <c:v>84.938488916882406</c:v>
                   </c:pt>
                   <c:pt idx="58">
-                    <c:v>100.78946705880399</c:v>
+                    <c:v>83.731193285324593</c:v>
                   </c:pt>
                   <c:pt idx="59">
-                    <c:v>99.689668061715196</c:v>
+                    <c:v>83.221774284760798</c:v>
                   </c:pt>
                   <c:pt idx="60">
-                    <c:v>103.516594224153</c:v>
+                    <c:v>84.203290393247201</c:v>
                   </c:pt>
                   <c:pt idx="61">
-                    <c:v>95.759293716147297</c:v>
+                    <c:v>82.057665337044995</c:v>
                   </c:pt>
                   <c:pt idx="62">
-                    <c:v>100.387918098631</c:v>
+                    <c:v>82.665659158335401</c:v>
                   </c:pt>
                   <c:pt idx="63">
-                    <c:v>97.261723203409204</c:v>
+                    <c:v>81.766857573413603</c:v>
                   </c:pt>
                   <c:pt idx="64">
-                    <c:v>101.22072392242499</c:v>
+                    <c:v>88.249724968299603</c:v>
                   </c:pt>
                   <c:pt idx="65">
-                    <c:v>102.002803578315</c:v>
+                    <c:v>84.647924673243196</c:v>
                   </c:pt>
                   <c:pt idx="66">
-                    <c:v>100.892933790336</c:v>
+                    <c:v>87.910430936452698</c:v>
                   </c:pt>
                   <c:pt idx="67">
-                    <c:v>99.381532000379806</c:v>
+                    <c:v>85.906475062918304</c:v>
                   </c:pt>
                   <c:pt idx="68">
-                    <c:v>103.943241126937</c:v>
+                    <c:v>84.768727843478203</c:v>
                   </c:pt>
                   <c:pt idx="69">
-                    <c:v>99.2999859174204</c:v>
+                    <c:v>85.191755519779093</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -846,214 +846,214 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="0">
-                  <c:v>-21.879308409775401</c:v>
+                  <c:v>3.2775865056244</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-15.1687439168112</c:v>
+                  <c:v>1.9563420176614099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-13.444619014417601</c:v>
+                  <c:v>15.441073997985299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-20.8307830795322</c:v>
+                  <c:v>9.0246450995741103</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-19.711256867903199</c:v>
+                  <c:v>6.1228641423836798</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-22.6972964440568</c:v>
+                  <c:v>6.66810234947223</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-14.9374152031614</c:v>
+                  <c:v>6.6045220663341402</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-25.028163565863299</c:v>
+                  <c:v>7.0278744855232098</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-18.761707954455002</c:v>
+                  <c:v>7.79442514146099</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-21.1514540001425</c:v>
+                  <c:v>7.7940361147308597</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.951321088259601</c:v>
+                  <c:v>17.160757620059702</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-11.1270251671396</c:v>
+                  <c:v>2.30323092416445</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-20.6700906654028</c:v>
+                  <c:v>9.3672235700829098</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-22.765324323040598</c:v>
+                  <c:v>8.3577110781911994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-13.4641362189983</c:v>
+                  <c:v>7.3615690569842798</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-17.008824797142299</c:v>
+                  <c:v>9.8652041943560498</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-16.452143913326701</c:v>
+                  <c:v>6.8798503954145103</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-21.506662043467099</c:v>
+                  <c:v>9.32819835278681</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-22.3767095038944</c:v>
+                  <c:v>3.2811450360903498</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-20.794135165149601</c:v>
+                  <c:v>7.0691799053959201</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-11.335161434746899</c:v>
+                  <c:v>1.70233611314897</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-5.5053892179011301</c:v>
+                  <c:v>2.0105684396694499</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-19.341203957290901</c:v>
+                  <c:v>6.4646067261849103</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-21.043053357867901</c:v>
+                  <c:v>5.6161444418385003</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-15.6022128898235</c:v>
+                  <c:v>5.6230649588279302</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-25.753141379902999</c:v>
+                  <c:v>6.9370369208727398</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-12.915491096405701</c:v>
+                  <c:v>4.3447712828269802</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-19.019158099907301</c:v>
+                  <c:v>5.0109198654336202</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-14.8670858487147</c:v>
+                  <c:v>6.80015430026386</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-13.638777712152599</c:v>
+                  <c:v>9.5530199756009004</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-18.331558142575599</c:v>
+                  <c:v>4.9323298241342401</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-14.658918623058399</c:v>
+                  <c:v>5.6114236237519401</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-31.571668672103002</c:v>
+                  <c:v>3.2428014811832599</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-22.7820504335909</c:v>
+                  <c:v>3.7263194723924902</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-19.6085693323238</c:v>
+                  <c:v>5.0914299872168698</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-9.2257303168908393</c:v>
+                  <c:v>8.4415323722481208</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-17.258030775158002</c:v>
+                  <c:v>4.7986741304640699</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-15.474808642373601</c:v>
+                  <c:v>2.88750999447279</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-14.298383773585099</c:v>
+                  <c:v>6.4992756203712903</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-14.014931238951</c:v>
+                  <c:v>0.493700298804227</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-15.7325969945704</c:v>
+                  <c:v>7.7794780526687699</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-25.524705805754401</c:v>
+                  <c:v>9.1918765187565299</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-16.931923516207</c:v>
+                  <c:v>5.2377275672514596</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>13.7875503302879</c:v>
+                  <c:v>16.228085889245701</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-22.431295151115101</c:v>
+                  <c:v>13.5796053382913</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-10.9339321001607</c:v>
+                  <c:v>6.9428331868213897</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-19.853855260868901</c:v>
+                  <c:v>6.2103281089504403</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-19.711409046100801</c:v>
+                  <c:v>9.0699272828671198</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-19.084729813783898</c:v>
+                  <c:v>8.8620382367106192</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-19.3949735932595</c:v>
+                  <c:v>8.4061789338097093</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-18.325283864361701</c:v>
+                  <c:v>7.7383268540597596</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-20.637855995020299</c:v>
+                  <c:v>8.5983857920934792</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-19.0506999946919</c:v>
+                  <c:v>9.4980006870852502</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-15.530030172791401</c:v>
+                  <c:v>5.4720943727583098</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-23.9083726969019</c:v>
+                  <c:v>9.5373024287048196</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>14.033252344738701</c:v>
+                  <c:v>21.611876570439801</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-26.778140959439</c:v>
+                  <c:v>5.02784863138824</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-22.495404674465298</c:v>
+                  <c:v>8.7103858855391607</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-8.37267523636676</c:v>
+                  <c:v>6.8268979056296804</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-23.116206488230901</c:v>
+                  <c:v>5.6312994227368502</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-9.2578279084223105</c:v>
+                  <c:v>6.9171130076183402</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-19.1858704085573</c:v>
+                  <c:v>8.3781325405889895</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-22.781945871886901</c:v>
+                  <c:v>9.7085486362762303</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-20.176691910534501</c:v>
+                  <c:v>6.2745586685752999</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>-15.2866903993181</c:v>
+                  <c:v>1.9809189310256401</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-15.3161898308483</c:v>
+                  <c:v>4.3987242224592604</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-10.708513690779499</c:v>
+                  <c:v>2.1980318800568499</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-15.5715269124284</c:v>
+                  <c:v>7.1118124073843303</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-15.1547660725781</c:v>
+                  <c:v>4.1439922202397996</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-15.668777898903199</c:v>
+                  <c:v>4.16248115299953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1130,214 +1130,214 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="70"/>
                   <c:pt idx="0">
-                    <c:v>8.86910061871626</c:v>
+                    <c:v>9.1557196913139105</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>9.2541180316795906</c:v>
+                    <c:v>8.9593290947085595</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.0076681227918396</c:v>
+                    <c:v>6.6553985682076897</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.4717840908530597</c:v>
+                    <c:v>6.9752969180463902</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.1724295200944104</c:v>
+                    <c:v>6.6212222295908196</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>7.6394064052042996</c:v>
+                    <c:v>7.1209508957957404</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>6.9681371464399504</c:v>
+                    <c:v>6.6919460115816101</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>8.0202893525843706</c:v>
+                    <c:v>7.8217375252861503</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.4147883465822604</c:v>
+                    <c:v>7.1308962698676996</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>7.2400187498049799</c:v>
+                    <c:v>6.9421747967827496</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>112.80707952471499</c:v>
+                    <c:v>115.597280052011</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>9.4491383987289996</c:v>
+                    <c:v>7.1597568638129303</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>10.083924021460501</c:v>
+                    <c:v>7.49199388175255</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>10.6899862762809</c:v>
+                    <c:v>7.2057397601797799</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>10.4944275157044</c:v>
+                    <c:v>6.8805428432386098</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>10.8259630445847</c:v>
+                    <c:v>7.0489170240646102</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>10.0158060050193</c:v>
+                    <c:v>6.6491364697332402</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>9.6981709407377998</c:v>
+                    <c:v>7.2634375817477004</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>9.5463845287664206</c:v>
+                    <c:v>7.3766521268915</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>10.6340145623236</c:v>
+                    <c:v>7.4837608722249298</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>9.7799984040560606</c:v>
+                    <c:v>9.2611530750372406</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>7.3975113429131998</c:v>
+                    <c:v>7.3457768957184104</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>6.8474200009566797</c:v>
+                    <c:v>6.9711027275569499</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>7.6908275820509999</c:v>
+                    <c:v>7.0275307761719104</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>6.8953462661279499</c:v>
+                    <c:v>6.6982321594624503</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>7.2797014394130999</c:v>
+                    <c:v>7.2899002437381997</c:v>
                   </c:pt>
                   <c:pt idx="26">
-                    <c:v>6.9306207550275802</c:v>
+                    <c:v>6.6035609630034102</c:v>
                   </c:pt>
                   <c:pt idx="27">
-                    <c:v>7.57379051192778</c:v>
+                    <c:v>7.2067185732551202</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>7.2724634834249704</c:v>
+                    <c:v>6.8628459103739301</c:v>
                   </c:pt>
                   <c:pt idx="29">
-                    <c:v>8.0162508562550308</c:v>
+                    <c:v>8.2999661806778704</c:v>
                   </c:pt>
                   <c:pt idx="30">
-                    <c:v>9.0749775657593599</c:v>
+                    <c:v>8.5483897300556997</c:v>
                   </c:pt>
                   <c:pt idx="31">
-                    <c:v>7.21741650992029</c:v>
+                    <c:v>7.6359199206035999</c:v>
                   </c:pt>
                   <c:pt idx="32">
-                    <c:v>7.4547464743827598</c:v>
+                    <c:v>6.8117651679934497</c:v>
                   </c:pt>
                   <c:pt idx="33">
-                    <c:v>7.2052390346724202</c:v>
+                    <c:v>6.8567408122054596</c:v>
                   </c:pt>
                   <c:pt idx="34">
-                    <c:v>5.1899022033482201</c:v>
+                    <c:v>4.9793825008240997</c:v>
                   </c:pt>
                   <c:pt idx="35">
-                    <c:v>6.7250131854770103</c:v>
+                    <c:v>6.5764268243630104</c:v>
                   </c:pt>
                   <c:pt idx="36">
-                    <c:v>7.0976145715430103</c:v>
+                    <c:v>6.9415503165852304</c:v>
                   </c:pt>
                   <c:pt idx="37">
-                    <c:v>7.1801710952307598</c:v>
+                    <c:v>6.5045765021195798</c:v>
                   </c:pt>
                   <c:pt idx="38">
-                    <c:v>7.1949984340440798</c:v>
+                    <c:v>7.4759373094459898</c:v>
                   </c:pt>
                   <c:pt idx="39">
-                    <c:v>7.3531315651561497</c:v>
+                    <c:v>6.8128777112709802</c:v>
                   </c:pt>
                   <c:pt idx="40">
-                    <c:v>9.2074420793101801</c:v>
+                    <c:v>8.7252210391280105</c:v>
                   </c:pt>
                   <c:pt idx="41">
-                    <c:v>7.3910605851766</c:v>
+                    <c:v>6.6853815753878099</c:v>
                   </c:pt>
                   <c:pt idx="42">
-                    <c:v>8.3286557522071707</c:v>
+                    <c:v>7.0924566502506803</c:v>
                   </c:pt>
                   <c:pt idx="43">
-                    <c:v>114.541229089569</c:v>
+                    <c:v>113.273392492122</c:v>
                   </c:pt>
                   <c:pt idx="44">
-                    <c:v>7.27476917028764</c:v>
+                    <c:v>7.07779082913581</c:v>
                   </c:pt>
                   <c:pt idx="45">
-                    <c:v>7.6489288557822501</c:v>
+                    <c:v>7.2629181083531202</c:v>
                   </c:pt>
                   <c:pt idx="46">
-                    <c:v>7.4881588455203802</c:v>
+                    <c:v>6.8292318625129296</c:v>
                   </c:pt>
                   <c:pt idx="47">
-                    <c:v>8.1279337283375206</c:v>
+                    <c:v>7.6687770753459201</c:v>
                   </c:pt>
                   <c:pt idx="48">
-                    <c:v>7.4488978979828904</c:v>
+                    <c:v>7.3758417435021304</c:v>
                   </c:pt>
                   <c:pt idx="49">
-                    <c:v>7.15494037112905</c:v>
+                    <c:v>6.6527631497801902</c:v>
                   </c:pt>
                   <c:pt idx="50">
-                    <c:v>9.8320274870092899</c:v>
+                    <c:v>8.8071898396000297</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>7.2228911935213098</c:v>
+                    <c:v>7.0106924283953704</c:v>
                   </c:pt>
                   <c:pt idx="52">
-                    <c:v>7.5682032070265501</c:v>
+                    <c:v>6.8779291288537001</c:v>
                   </c:pt>
                   <c:pt idx="53">
-                    <c:v>7.9557750046834501</c:v>
+                    <c:v>7.10121532475985</c:v>
                   </c:pt>
                   <c:pt idx="54">
-                    <c:v>8.3659867354087893</c:v>
+                    <c:v>7.4835268368554804</c:v>
                   </c:pt>
                   <c:pt idx="55">
-                    <c:v>110.92038157853101</c:v>
+                    <c:v>113.394608277892</c:v>
                   </c:pt>
                   <c:pt idx="56">
-                    <c:v>9.1897741264566299</c:v>
+                    <c:v>8.3393061641596606</c:v>
                   </c:pt>
                   <c:pt idx="57">
-                    <c:v>7.7270538001747502</c:v>
+                    <c:v>7.2080471661763204</c:v>
                   </c:pt>
                   <c:pt idx="58">
-                    <c:v>7.9307410168293497</c:v>
+                    <c:v>7.1080924969268597</c:v>
                   </c:pt>
                   <c:pt idx="59">
-                    <c:v>7.5163162711801901</c:v>
+                    <c:v>6.9776163730675496</c:v>
                   </c:pt>
                   <c:pt idx="60">
-                    <c:v>9.0504121292515904</c:v>
+                    <c:v>9.0898169594069191</c:v>
                   </c:pt>
                   <c:pt idx="61">
-                    <c:v>7.4459831426556899</c:v>
+                    <c:v>7.8612060546373099</c:v>
                   </c:pt>
                   <c:pt idx="62">
-                    <c:v>7.0591479863220101</c:v>
+                    <c:v>6.6863359680894696</c:v>
                   </c:pt>
                   <c:pt idx="63">
-                    <c:v>6.9130388247678498</c:v>
+                    <c:v>7.1985780882947497</c:v>
                   </c:pt>
                   <c:pt idx="64">
-                    <c:v>9.5718394642682902</c:v>
+                    <c:v>6.9559301645901996</c:v>
                   </c:pt>
                   <c:pt idx="65">
-                    <c:v>10.017230874818701</c:v>
+                    <c:v>8.4890613648070801</c:v>
                   </c:pt>
                   <c:pt idx="66">
-                    <c:v>7.3254622756469097</c:v>
+                    <c:v>7.1810157075207801</c:v>
                   </c:pt>
                   <c:pt idx="67">
-                    <c:v>7.3825457342209004</c:v>
+                    <c:v>7.1513240160204496</c:v>
                   </c:pt>
                   <c:pt idx="68">
-                    <c:v>6.9219037288253098</c:v>
+                    <c:v>6.8665736988166097</c:v>
                   </c:pt>
                   <c:pt idx="69">
-                    <c:v>7.2340184212317098</c:v>
+                    <c:v>6.9367770229960604</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1349,214 +1349,214 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="70"/>
                   <c:pt idx="0">
-                    <c:v>8.86910061871626</c:v>
+                    <c:v>9.1557196913139105</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>9.2541180316795906</c:v>
+                    <c:v>8.9593290947085595</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.0076681227918396</c:v>
+                    <c:v>6.6553985682076897</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.4717840908530597</c:v>
+                    <c:v>6.9752969180463902</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.1724295200944104</c:v>
+                    <c:v>6.6212222295908196</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>7.6394064052042996</c:v>
+                    <c:v>7.1209508957957404</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>6.9681371464399504</c:v>
+                    <c:v>6.6919460115816101</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>8.0202893525843706</c:v>
+                    <c:v>7.8217375252861503</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.4147883465822604</c:v>
+                    <c:v>7.1308962698676996</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>7.2400187498049799</c:v>
+                    <c:v>6.9421747967827496</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>112.80707952471499</c:v>
+                    <c:v>115.597280052011</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>9.4491383987289996</c:v>
+                    <c:v>7.1597568638129303</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>10.083924021460501</c:v>
+                    <c:v>7.49199388175255</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>10.6899862762809</c:v>
+                    <c:v>7.2057397601797799</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>10.4944275157044</c:v>
+                    <c:v>6.8805428432386098</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>10.8259630445847</c:v>
+                    <c:v>7.0489170240646102</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>10.0158060050193</c:v>
+                    <c:v>6.6491364697332402</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>9.6981709407377998</c:v>
+                    <c:v>7.2634375817477004</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>9.5463845287664206</c:v>
+                    <c:v>7.3766521268915</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>10.6340145623236</c:v>
+                    <c:v>7.4837608722249298</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>9.7799984040560606</c:v>
+                    <c:v>9.2611530750372406</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>7.3975113429131998</c:v>
+                    <c:v>7.3457768957184104</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>6.8474200009566797</c:v>
+                    <c:v>6.9711027275569499</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>7.6908275820509999</c:v>
+                    <c:v>7.0275307761719104</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>6.8953462661279499</c:v>
+                    <c:v>6.6982321594624503</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>7.2797014394130999</c:v>
+                    <c:v>7.2899002437381997</c:v>
                   </c:pt>
                   <c:pt idx="26">
-                    <c:v>6.9306207550275802</c:v>
+                    <c:v>6.6035609630034102</c:v>
                   </c:pt>
                   <c:pt idx="27">
-                    <c:v>7.57379051192778</c:v>
+                    <c:v>7.2067185732551202</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>7.2724634834249704</c:v>
+                    <c:v>6.8628459103739301</c:v>
                   </c:pt>
                   <c:pt idx="29">
-                    <c:v>8.0162508562550308</c:v>
+                    <c:v>8.2999661806778704</c:v>
                   </c:pt>
                   <c:pt idx="30">
-                    <c:v>9.0749775657593599</c:v>
+                    <c:v>8.5483897300556997</c:v>
                   </c:pt>
                   <c:pt idx="31">
-                    <c:v>7.21741650992029</c:v>
+                    <c:v>7.6359199206035999</c:v>
                   </c:pt>
                   <c:pt idx="32">
-                    <c:v>7.4547464743827598</c:v>
+                    <c:v>6.8117651679934497</c:v>
                   </c:pt>
                   <c:pt idx="33">
-                    <c:v>7.2052390346724202</c:v>
+                    <c:v>6.8567408122054596</c:v>
                   </c:pt>
                   <c:pt idx="34">
-                    <c:v>5.1899022033482201</c:v>
+                    <c:v>4.9793825008240997</c:v>
                   </c:pt>
                   <c:pt idx="35">
-                    <c:v>6.7250131854770103</c:v>
+                    <c:v>6.5764268243630104</c:v>
                   </c:pt>
                   <c:pt idx="36">
-                    <c:v>7.0976145715430103</c:v>
+                    <c:v>6.9415503165852304</c:v>
                   </c:pt>
                   <c:pt idx="37">
-                    <c:v>7.1801710952307598</c:v>
+                    <c:v>6.5045765021195798</c:v>
                   </c:pt>
                   <c:pt idx="38">
-                    <c:v>7.1949984340440798</c:v>
+                    <c:v>7.4759373094459898</c:v>
                   </c:pt>
                   <c:pt idx="39">
-                    <c:v>7.3531315651561497</c:v>
+                    <c:v>6.8128777112709802</c:v>
                   </c:pt>
                   <c:pt idx="40">
-                    <c:v>9.2074420793101801</c:v>
+                    <c:v>8.7252210391280105</c:v>
                   </c:pt>
                   <c:pt idx="41">
-                    <c:v>7.3910605851766</c:v>
+                    <c:v>6.6853815753878099</c:v>
                   </c:pt>
                   <c:pt idx="42">
-                    <c:v>8.3286557522071707</c:v>
+                    <c:v>7.0924566502506803</c:v>
                   </c:pt>
                   <c:pt idx="43">
-                    <c:v>114.541229089569</c:v>
+                    <c:v>113.273392492122</c:v>
                   </c:pt>
                   <c:pt idx="44">
-                    <c:v>7.27476917028764</c:v>
+                    <c:v>7.07779082913581</c:v>
                   </c:pt>
                   <c:pt idx="45">
-                    <c:v>7.6489288557822501</c:v>
+                    <c:v>7.2629181083531202</c:v>
                   </c:pt>
                   <c:pt idx="46">
-                    <c:v>7.4881588455203802</c:v>
+                    <c:v>6.8292318625129296</c:v>
                   </c:pt>
                   <c:pt idx="47">
-                    <c:v>8.1279337283375206</c:v>
+                    <c:v>7.6687770753459201</c:v>
                   </c:pt>
                   <c:pt idx="48">
-                    <c:v>7.4488978979828904</c:v>
+                    <c:v>7.3758417435021304</c:v>
                   </c:pt>
                   <c:pt idx="49">
-                    <c:v>7.15494037112905</c:v>
+                    <c:v>6.6527631497801902</c:v>
                   </c:pt>
                   <c:pt idx="50">
-                    <c:v>9.8320274870092899</c:v>
+                    <c:v>8.8071898396000297</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>7.2228911935213098</c:v>
+                    <c:v>7.0106924283953704</c:v>
                   </c:pt>
                   <c:pt idx="52">
-                    <c:v>7.5682032070265501</c:v>
+                    <c:v>6.8779291288537001</c:v>
                   </c:pt>
                   <c:pt idx="53">
-                    <c:v>7.9557750046834501</c:v>
+                    <c:v>7.10121532475985</c:v>
                   </c:pt>
                   <c:pt idx="54">
-                    <c:v>8.3659867354087893</c:v>
+                    <c:v>7.4835268368554804</c:v>
                   </c:pt>
                   <c:pt idx="55">
-                    <c:v>110.92038157853101</c:v>
+                    <c:v>113.394608277892</c:v>
                   </c:pt>
                   <c:pt idx="56">
-                    <c:v>9.1897741264566299</c:v>
+                    <c:v>8.3393061641596606</c:v>
                   </c:pt>
                   <c:pt idx="57">
-                    <c:v>7.7270538001747502</c:v>
+                    <c:v>7.2080471661763204</c:v>
                   </c:pt>
                   <c:pt idx="58">
-                    <c:v>7.9307410168293497</c:v>
+                    <c:v>7.1080924969268597</c:v>
                   </c:pt>
                   <c:pt idx="59">
-                    <c:v>7.5163162711801901</c:v>
+                    <c:v>6.9776163730675496</c:v>
                   </c:pt>
                   <c:pt idx="60">
-                    <c:v>9.0504121292515904</c:v>
+                    <c:v>9.0898169594069191</c:v>
                   </c:pt>
                   <c:pt idx="61">
-                    <c:v>7.4459831426556899</c:v>
+                    <c:v>7.8612060546373099</c:v>
                   </c:pt>
                   <c:pt idx="62">
-                    <c:v>7.0591479863220101</c:v>
+                    <c:v>6.6863359680894696</c:v>
                   </c:pt>
                   <c:pt idx="63">
-                    <c:v>6.9130388247678498</c:v>
+                    <c:v>7.1985780882947497</c:v>
                   </c:pt>
                   <c:pt idx="64">
-                    <c:v>9.5718394642682902</c:v>
+                    <c:v>6.9559301645901996</c:v>
                   </c:pt>
                   <c:pt idx="65">
-                    <c:v>10.017230874818701</c:v>
+                    <c:v>8.4890613648070801</c:v>
                   </c:pt>
                   <c:pt idx="66">
-                    <c:v>7.3254622756469097</c:v>
+                    <c:v>7.1810157075207801</c:v>
                   </c:pt>
                   <c:pt idx="67">
-                    <c:v>7.3825457342209004</c:v>
+                    <c:v>7.1513240160204496</c:v>
                   </c:pt>
                   <c:pt idx="68">
-                    <c:v>6.9219037288253098</c:v>
+                    <c:v>6.8665736988166097</c:v>
                   </c:pt>
                   <c:pt idx="69">
-                    <c:v>7.2340184212317098</c:v>
+                    <c:v>6.9367770229960604</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1798,214 +1798,214 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="0">
-                  <c:v>-0.67480442150025799</c:v>
+                  <c:v>-9.5941958597619198E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.0269466022928599</c:v>
+                  <c:v>-0.15590019222523199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.23903079687425999</c:v>
+                  <c:v>-9.9030288687485896E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.33842110022133298</c:v>
+                  <c:v>-4.3768231535389703E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.317442766948627</c:v>
+                  <c:v>-9.3017857305034105E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.15141292289878699</c:v>
+                  <c:v>-0.36995598863789603</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.24609093388745201</c:v>
+                  <c:v>-4.2000334837748399E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.44227928016965801</c:v>
+                  <c:v>4.0673878435380402E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.53270387389555296</c:v>
+                  <c:v>2.55900609083793E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.18893985495649701</c:v>
+                  <c:v>4.0194092975607103E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.951321088259601</c:v>
+                  <c:v>17.160757620059702</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.9976512722361804E-2</c:v>
+                  <c:v>-3.15697729701028E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.82846144504806496</c:v>
+                  <c:v>-0.197936710513411</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.7743700636292901E-2</c:v>
+                  <c:v>-5.7923770123635499E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.53654529570833598</c:v>
+                  <c:v>-0.10202603670843299</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.16465752925150701</c:v>
+                  <c:v>-1.47624137420074E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.79721492918581405</c:v>
+                  <c:v>0.17284503301263801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.22627996012175799</c:v>
+                  <c:v>7.9575199874418995E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.16264373343525201</c:v>
+                  <c:v>-0.178310464142755</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-6.3107145247597897E-3</c:v>
+                  <c:v>-0.15985939985049899</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.45303041729117399</c:v>
+                  <c:v>-5.1999764474526901E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.1849629682650998E-2</c:v>
+                  <c:v>-4.1503796115278303E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.183505039258713</c:v>
+                  <c:v>-3.1567576900513698E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.15184102935461399</c:v>
+                  <c:v>7.0222310435943402E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.46485529494838901</c:v>
+                  <c:v>0.193353351808107</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.224036673458017</c:v>
+                  <c:v>0.21635721617870099</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-5.91898388967977E-2</c:v>
+                  <c:v>0.12689859302881601</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.18092771407799699</c:v>
+                  <c:v>-5.7195050503553203E-3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-3.4833803406881698E-2</c:v>
+                  <c:v>3.6537548264644298E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.14529880118921101</c:v>
+                  <c:v>-0.15430850763301901</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.624982706427891</c:v>
+                  <c:v>0.290462114304261</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-0.122180171371139</c:v>
+                  <c:v>0.20321232582530099</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-0.19877434388447199</c:v>
+                  <c:v>-0.220058715211774</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.246867377305129</c:v>
+                  <c:v>8.2234263454331505E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.16145219984305101</c:v>
+                  <c:v>9.6268170001946402E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.4065313272510499E-2</c:v>
+                  <c:v>2.26268123083583E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.102086544044641</c:v>
+                  <c:v>-9.9916421229870406E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.14096751365304599</c:v>
+                  <c:v>-4.7971065312090798E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.35622785817279601</c:v>
+                  <c:v>0.36416893777147902</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.1420623257381303E-3</c:v>
+                  <c:v>0.16016145763959599</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-0.39272586870412302</c:v>
+                  <c:v>-5.1967330009927998E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.70949087345576E-2</c:v>
+                  <c:v>-5.2323029988585998E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-8.1763018883805397E-2</c:v>
+                  <c:v>-0.12262279068084</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>13.7875503302879</c:v>
+                  <c:v>16.228085889245701</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>7.4381454833878202E-2</c:v>
+                  <c:v>-3.88250378421141E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.1369658717116703E-2</c:v>
+                  <c:v>6.4716568259429605E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-6.8929007868546499E-2</c:v>
+                  <c:v>-6.0228253343145501E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-0.14358012969970099</c:v>
+                  <c:v>6.2070350961409802E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.8937385955307999E-2</c:v>
+                  <c:v>4.1632453634239099E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.11693285621157599</c:v>
+                  <c:v>-7.49499958356213E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-0.55709555613941197</c:v>
+                  <c:v>-0.19148575083399599</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-0.14148662127575601</c:v>
+                  <c:v>9.7787103508706799E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-3.3230783032679401E-2</c:v>
+                  <c:v>-0.17279151207134999</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-7.3190901221677096E-2</c:v>
+                  <c:v>8.4370252879750807E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.215403077516404</c:v>
+                  <c:v>0.12732271998674</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>14.033252344738701</c:v>
+                  <c:v>21.611876570439801</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-2.74534290043057E-2</c:v>
+                  <c:v>0.477429364781007</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.5960212607275599E-2</c:v>
+                  <c:v>-1.4650697166731501E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-0.28820596460929498</c:v>
+                  <c:v>9.5595884192418101E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-0.24453810465273601</c:v>
+                  <c:v>-0.209934931215112</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-0.88119796433714004</c:v>
+                  <c:v>0.21586708934842799</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-0.25666580650536203</c:v>
+                  <c:v>-0.36635347540393898</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-0.21671397065065801</c:v>
+                  <c:v>7.2977281185312897E-3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-0.19880524101407199</c:v>
+                  <c:v>-0.186007520924898</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.8245481247918999E-2</c:v>
+                  <c:v>-7.4661853894276195E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-0.23813335425746199</c:v>
+                  <c:v>0.34284608474920503</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-0.23186909464914901</c:v>
+                  <c:v>-0.10204368137683401</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-0.35115536855915103</c:v>
+                  <c:v>2.7118101010553501E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-0.24311345663230599</c:v>
+                  <c:v>-0.13780831920132799</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-0.413431139582769</c:v>
+                  <c:v>0.13224299031846001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2020,11 +2020,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="271946160"/>
-        <c:axId val="271948880"/>
+        <c:axId val="-1406434832"/>
+        <c:axId val="-1406432656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="271946160"/>
+        <c:axId val="-1406434832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -2138,12 +2138,12 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="271948880"/>
+        <c:crossAx val="-1406432656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="271948880"/>
+        <c:axId val="-1406432656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2256,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="271946160"/>
+        <c:crossAx val="-1406434832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3220,7 +3220,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E71"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3247,16 +3247,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-21.879308409775401</v>
+        <v>3.2775865056244</v>
       </c>
       <c r="C2">
-        <v>104.838671306191</v>
+        <v>85.051000068270596</v>
       </c>
       <c r="D2">
-        <v>-0.67480442150025799</v>
+        <v>-9.5941958597619198E-2</v>
       </c>
       <c r="E2">
-        <v>8.86910061871626</v>
+        <v>9.1557196913139105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -3264,16 +3264,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-15.1687439168112</v>
+        <v>1.9563420176614099</v>
       </c>
       <c r="C3">
-        <v>102.29111208984</v>
+        <v>83.545042422626196</v>
       </c>
       <c r="D3">
-        <v>-1.0269466022928599</v>
+        <v>-0.15590019222523199</v>
       </c>
       <c r="E3">
-        <v>9.2541180316795906</v>
+        <v>8.9593290947085595</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3281,16 +3281,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-13.444619014417601</v>
+        <v>15.441073997985299</v>
       </c>
       <c r="C4">
-        <v>102.05013617433799</v>
+        <v>82.776149638236106</v>
       </c>
       <c r="D4">
-        <v>-0.23903079687425999</v>
+        <v>-9.9030288687485896E-2</v>
       </c>
       <c r="E4">
-        <v>7.0076681227918396</v>
+        <v>6.6553985682076897</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3298,16 +3298,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-20.8307830795322</v>
+        <v>9.0246450995741103</v>
       </c>
       <c r="C5">
-        <v>100.842466787677</v>
+        <v>82.624740075180995</v>
       </c>
       <c r="D5">
-        <v>-0.33842110022133298</v>
+        <v>-4.3768231535389703E-2</v>
       </c>
       <c r="E5">
-        <v>7.4717840908530597</v>
+        <v>6.9752969180463902</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -3315,16 +3315,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-19.711256867903199</v>
+        <v>6.1228641423836798</v>
       </c>
       <c r="C6">
-        <v>100.565405933363</v>
+        <v>86.304328143395395</v>
       </c>
       <c r="D6">
-        <v>-0.317442766948627</v>
+        <v>-9.3017857305034105E-2</v>
       </c>
       <c r="E6">
-        <v>7.1724295200944104</v>
+        <v>6.6212222295908196</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3332,16 +3332,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-22.6972964440568</v>
+        <v>6.66810234947223</v>
       </c>
       <c r="C7">
-        <v>99.425776980452397</v>
+        <v>81.237954199280907</v>
       </c>
       <c r="D7">
-        <v>-0.15141292289878699</v>
+        <v>-0.36995598863789603</v>
       </c>
       <c r="E7">
-        <v>7.6394064052042996</v>
+        <v>7.1209508957957404</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3349,16 +3349,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-14.9374152031614</v>
+        <v>6.6045220663341402</v>
       </c>
       <c r="C8">
-        <v>99.391387237600796</v>
+        <v>82.225810410563099</v>
       </c>
       <c r="D8">
-        <v>-0.24609093388745201</v>
+        <v>-4.2000334837748399E-2</v>
       </c>
       <c r="E8">
-        <v>6.9681371464399504</v>
+        <v>6.6919460115816101</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3366,16 +3366,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-25.028163565863299</v>
+        <v>7.0278744855232098</v>
       </c>
       <c r="C9">
-        <v>98.497121431295895</v>
+        <v>85.792131824098703</v>
       </c>
       <c r="D9">
-        <v>-0.44227928016965801</v>
+        <v>4.0673878435380402E-2</v>
       </c>
       <c r="E9">
-        <v>8.0202893525843706</v>
+        <v>7.8217375252861503</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -3383,16 +3383,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-18.761707954455002</v>
+        <v>7.79442514146099</v>
       </c>
       <c r="C10">
-        <v>99.495419745672095</v>
+        <v>86.506323016713594</v>
       </c>
       <c r="D10">
-        <v>-0.53270387389555296</v>
+        <v>2.55900609083793E-3</v>
       </c>
       <c r="E10">
-        <v>7.4147883465822604</v>
+        <v>7.1308962698676996</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -3400,16 +3400,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-21.1514540001425</v>
+        <v>7.7940361147308597</v>
       </c>
       <c r="C11">
-        <v>100.16072469089499</v>
+        <v>81.8971269724519</v>
       </c>
       <c r="D11">
-        <v>-0.18893985495649701</v>
+        <v>4.0194092975607103E-2</v>
       </c>
       <c r="E11">
-        <v>7.2400187498049799</v>
+        <v>6.9421747967827496</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -3417,16 +3417,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>22.951321088259601</v>
+        <v>17.160757620059702</v>
       </c>
       <c r="C12">
-        <v>112.80707952471499</v>
+        <v>115.597280052011</v>
       </c>
       <c r="D12">
-        <v>22.951321088259601</v>
+        <v>17.160757620059702</v>
       </c>
       <c r="E12">
-        <v>112.80707952471499</v>
+        <v>115.597280052011</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -3434,16 +3434,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-11.1270251671396</v>
+        <v>2.30323092416445</v>
       </c>
       <c r="C13">
-        <v>100.671111382531</v>
+        <v>84.051944619351104</v>
       </c>
       <c r="D13">
-        <v>8.9976512722361804E-2</v>
+        <v>-3.15697729701028E-2</v>
       </c>
       <c r="E13">
-        <v>9.4491383987289996</v>
+        <v>7.1597568638129303</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -3451,16 +3451,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-20.6700906654028</v>
+        <v>9.3672235700829098</v>
       </c>
       <c r="C14">
-        <v>101.013391876486</v>
+        <v>82.548378261890406</v>
       </c>
       <c r="D14">
-        <v>-0.82846144504806496</v>
+        <v>-0.197936710513411</v>
       </c>
       <c r="E14">
-        <v>10.083924021460501</v>
+        <v>7.49199388175255</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -3468,16 +3468,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-22.765324323040598</v>
+        <v>8.3577110781911994</v>
       </c>
       <c r="C15">
-        <v>97.943175694066497</v>
+        <v>83.400048488353505</v>
       </c>
       <c r="D15">
-        <v>8.7743700636292901E-2</v>
+        <v>-5.7923770123635499E-3</v>
       </c>
       <c r="E15">
-        <v>10.6899862762809</v>
+        <v>7.2057397601797799</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -3485,16 +3485,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-13.4641362189983</v>
+        <v>7.3615690569842798</v>
       </c>
       <c r="C16">
-        <v>98.3888271217143</v>
+        <v>83.124704459000995</v>
       </c>
       <c r="D16">
-        <v>-0.53654529570833598</v>
+        <v>-0.10202603670843299</v>
       </c>
       <c r="E16">
-        <v>10.4944275157044</v>
+        <v>6.8805428432386098</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -3502,16 +3502,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-17.008824797142299</v>
+        <v>9.8652041943560498</v>
       </c>
       <c r="C17">
-        <v>99.069619310494801</v>
+        <v>84.894276343970702</v>
       </c>
       <c r="D17">
-        <v>0.16465752925150701</v>
+        <v>-1.47624137420074E-2</v>
       </c>
       <c r="E17">
-        <v>10.8259630445847</v>
+        <v>7.0489170240646102</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -3519,16 +3519,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-16.452143913326701</v>
+        <v>6.8798503954145103</v>
       </c>
       <c r="C18">
-        <v>96.927833873323607</v>
+        <v>83.485936866112894</v>
       </c>
       <c r="D18">
-        <v>-0.79721492918581405</v>
+        <v>0.17284503301263801</v>
       </c>
       <c r="E18">
-        <v>10.0158060050193</v>
+        <v>6.6491364697332402</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3536,16 +3536,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-21.506662043467099</v>
+        <v>9.32819835278681</v>
       </c>
       <c r="C19">
-        <v>102.26012677997301</v>
+        <v>85.363057623032105</v>
       </c>
       <c r="D19">
-        <v>0.22627996012175799</v>
+        <v>7.9575199874418995E-2</v>
       </c>
       <c r="E19">
-        <v>9.6981709407377998</v>
+        <v>7.2634375817477004</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -3553,16 +3553,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-22.3767095038944</v>
+        <v>3.2811450360903498</v>
       </c>
       <c r="C20">
-        <v>97.490487164652393</v>
+        <v>86.086235312413294</v>
       </c>
       <c r="D20">
-        <v>0.16264373343525201</v>
+        <v>-0.178310464142755</v>
       </c>
       <c r="E20">
-        <v>9.5463845287664206</v>
+        <v>7.3766521268915</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -3570,16 +3570,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-20.794135165149601</v>
+        <v>7.0691799053959201</v>
       </c>
       <c r="C21">
-        <v>96.201514272612798</v>
+        <v>85.502794142896605</v>
       </c>
       <c r="D21">
-        <v>-6.3107145247597897E-3</v>
+        <v>-0.15985939985049899</v>
       </c>
       <c r="E21">
-        <v>10.6340145623236</v>
+        <v>7.4837608722249298</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -3587,16 +3587,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-11.335161434746899</v>
+        <v>1.70233611314897</v>
       </c>
       <c r="C22">
-        <v>101.99076581904301</v>
+        <v>84.815465449479007</v>
       </c>
       <c r="D22">
-        <v>-0.45303041729117399</v>
+        <v>-5.1999764474526901E-2</v>
       </c>
       <c r="E22">
-        <v>9.7799984040560606</v>
+        <v>9.2611530750372406</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -3604,16 +3604,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-5.5053892179011301</v>
+        <v>2.0105684396694499</v>
       </c>
       <c r="C23">
-        <v>99.709325381999804</v>
+        <v>83.756172733130398</v>
       </c>
       <c r="D23">
-        <v>4.1849629682650998E-2</v>
+        <v>-4.1503796115278303E-2</v>
       </c>
       <c r="E23">
-        <v>7.3975113429131998</v>
+        <v>7.3457768957184104</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -3621,16 +3621,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>-19.341203957290901</v>
+        <v>6.4646067261849103</v>
       </c>
       <c r="C24">
-        <v>102.869996536557</v>
+        <v>84.629320475430802</v>
       </c>
       <c r="D24">
-        <v>-0.183505039258713</v>
+        <v>-3.1567576900513698E-2</v>
       </c>
       <c r="E24">
-        <v>6.8474200009566797</v>
+        <v>6.9711027275569499</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -3638,16 +3638,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>-21.043053357867901</v>
+        <v>5.6161444418385003</v>
       </c>
       <c r="C25">
-        <v>102.713694188217</v>
+        <v>84.291044484866006</v>
       </c>
       <c r="D25">
-        <v>-0.15184102935461399</v>
+        <v>7.0222310435943402E-2</v>
       </c>
       <c r="E25">
-        <v>7.6908275820509999</v>
+        <v>7.0275307761719104</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -3655,16 +3655,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-15.6022128898235</v>
+        <v>5.6230649588279302</v>
       </c>
       <c r="C26">
-        <v>97.4714040165113</v>
+        <v>85.284252007254494</v>
       </c>
       <c r="D26">
-        <v>-0.46485529494838901</v>
+        <v>0.193353351808107</v>
       </c>
       <c r="E26">
-        <v>6.8953462661279499</v>
+        <v>6.6982321594624503</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -3672,16 +3672,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-25.753141379902999</v>
+        <v>6.9370369208727398</v>
       </c>
       <c r="C27">
-        <v>100.811182367423</v>
+        <v>85.264297957082505</v>
       </c>
       <c r="D27">
-        <v>-0.224036673458017</v>
+        <v>0.21635721617870099</v>
       </c>
       <c r="E27">
-        <v>7.2797014394130999</v>
+        <v>7.2899002437381997</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -3689,16 +3689,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-12.915491096405701</v>
+        <v>4.3447712828269802</v>
       </c>
       <c r="C28">
-        <v>100.027118856602</v>
+        <v>83.069413889312102</v>
       </c>
       <c r="D28">
-        <v>-5.91898388967977E-2</v>
+        <v>0.12689859302881601</v>
       </c>
       <c r="E28">
-        <v>6.9306207550275802</v>
+        <v>6.6035609630034102</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -3706,16 +3706,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>-19.019158099907301</v>
+        <v>5.0109198654336202</v>
       </c>
       <c r="C29">
-        <v>96.221111702426498</v>
+        <v>85.509566945733297</v>
       </c>
       <c r="D29">
-        <v>-0.18092771407799699</v>
+        <v>-5.7195050503553203E-3</v>
       </c>
       <c r="E29">
-        <v>7.57379051192778</v>
+        <v>7.2067185732551202</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -3723,16 +3723,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>-14.8670858487147</v>
+        <v>6.80015430026386</v>
       </c>
       <c r="C30">
-        <v>100.318111756931</v>
+        <v>85.512167142847503</v>
       </c>
       <c r="D30">
-        <v>-3.4833803406881698E-2</v>
+        <v>3.6537548264644298E-3</v>
       </c>
       <c r="E30">
-        <v>7.2724634834249704</v>
+        <v>6.8628459103739301</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -3740,16 +3740,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>-13.638777712152599</v>
+        <v>9.5530199756009004</v>
       </c>
       <c r="C31">
-        <v>102.846837755156</v>
+        <v>83.493105784984493</v>
       </c>
       <c r="D31">
-        <v>-0.14529880118921101</v>
+        <v>-0.15430850763301901</v>
       </c>
       <c r="E31">
-        <v>8.0162508562550308</v>
+        <v>8.2999661806778704</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -3757,16 +3757,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>-18.331558142575599</v>
+        <v>4.9323298241342401</v>
       </c>
       <c r="C32">
-        <v>98.400686020703702</v>
+        <v>82.731672923523305</v>
       </c>
       <c r="D32">
-        <v>-0.624982706427891</v>
+        <v>0.290462114304261</v>
       </c>
       <c r="E32">
-        <v>9.0749775657593599</v>
+        <v>8.5483897300556997</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -3774,16 +3774,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>-14.658918623058399</v>
+        <v>5.6114236237519401</v>
       </c>
       <c r="C33">
-        <v>99.515041390427598</v>
+        <v>83.026084948991596</v>
       </c>
       <c r="D33">
-        <v>-0.122180171371139</v>
+        <v>0.20321232582530099</v>
       </c>
       <c r="E33">
-        <v>7.21741650992029</v>
+        <v>7.6359199206035999</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -3791,16 +3791,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>-31.571668672103002</v>
+        <v>3.2428014811832599</v>
       </c>
       <c r="C34">
-        <v>98.875548476422907</v>
+        <v>83.860137388589806</v>
       </c>
       <c r="D34">
-        <v>-0.19877434388447199</v>
+        <v>-0.220058715211774</v>
       </c>
       <c r="E34">
-        <v>7.4547464743827598</v>
+        <v>6.8117651679934497</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -3808,16 +3808,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>-22.7820504335909</v>
+        <v>3.7263194723924902</v>
       </c>
       <c r="C35">
-        <v>102.39863625739601</v>
+        <v>83.572044489308297</v>
       </c>
       <c r="D35">
-        <v>-0.246867377305129</v>
+        <v>8.2234263454331505E-2</v>
       </c>
       <c r="E35">
-        <v>7.2052390346724202</v>
+        <v>6.8567408122054596</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -3825,16 +3825,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>-19.6085693323238</v>
+        <v>5.0914299872168698</v>
       </c>
       <c r="C36">
-        <v>98.733556395947303</v>
+        <v>82.132281142149594</v>
       </c>
       <c r="D36">
-        <v>-0.16145219984305101</v>
+        <v>9.6268170001946402E-2</v>
       </c>
       <c r="E36">
-        <v>5.1899022033482201</v>
+        <v>4.9793825008240997</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -3842,16 +3842,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>-9.2257303168908393</v>
+        <v>8.4415323722481208</v>
       </c>
       <c r="C37">
-        <v>97.791815712052994</v>
+        <v>81.710724849113404</v>
       </c>
       <c r="D37">
-        <v>6.4065313272510499E-2</v>
+        <v>2.26268123083583E-2</v>
       </c>
       <c r="E37">
-        <v>6.7250131854770103</v>
+        <v>6.5764268243630104</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -3859,16 +3859,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>-17.258030775158002</v>
+        <v>4.7986741304640699</v>
       </c>
       <c r="C38">
-        <v>99.676727093416304</v>
+        <v>83.961438137922698</v>
       </c>
       <c r="D38">
-        <v>-0.102086544044641</v>
+        <v>-9.9916421229870406E-2</v>
       </c>
       <c r="E38">
-        <v>7.0976145715430103</v>
+        <v>6.9415503165852304</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -3876,16 +3876,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>-15.474808642373601</v>
+        <v>2.88750999447279</v>
       </c>
       <c r="C39">
-        <v>98.643907501151205</v>
+        <v>83.666107009785705</v>
       </c>
       <c r="D39">
-        <v>-0.14096751365304599</v>
+        <v>-4.7971065312090798E-2</v>
       </c>
       <c r="E39">
-        <v>7.1801710952307598</v>
+        <v>6.5045765021195798</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -3893,16 +3893,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>-14.298383773585099</v>
+        <v>6.4992756203712903</v>
       </c>
       <c r="C40">
-        <v>102.43705941507601</v>
+        <v>84.060798014025195</v>
       </c>
       <c r="D40">
-        <v>-0.35622785817279601</v>
+        <v>0.36416893777147902</v>
       </c>
       <c r="E40">
-        <v>7.1949984340440798</v>
+        <v>7.4759373094459898</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -3910,16 +3910,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>-14.014931238951</v>
+        <v>0.493700298804227</v>
       </c>
       <c r="C41">
-        <v>97.725078826283905</v>
+        <v>84.1053053152486</v>
       </c>
       <c r="D41">
-        <v>9.1420623257381303E-3</v>
+        <v>0.16016145763959599</v>
       </c>
       <c r="E41">
-        <v>7.3531315651561497</v>
+        <v>6.8128777112709802</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -3927,16 +3927,16 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>-15.7325969945704</v>
+        <v>7.7794780526687699</v>
       </c>
       <c r="C42">
-        <v>99.652085349332296</v>
+        <v>82.796274596050793</v>
       </c>
       <c r="D42">
-        <v>-0.39272586870412302</v>
+        <v>-5.1967330009927998E-3</v>
       </c>
       <c r="E42">
-        <v>9.2074420793101801</v>
+        <v>8.7252210391280105</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -3944,16 +3944,16 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>-25.524705805754401</v>
+        <v>9.1918765187565299</v>
       </c>
       <c r="C43">
-        <v>99.902023924803302</v>
+        <v>84.697772456638504</v>
       </c>
       <c r="D43">
-        <v>2.70949087345576E-2</v>
+        <v>-5.2323029988585998E-2</v>
       </c>
       <c r="E43">
-        <v>7.3910605851766</v>
+        <v>6.6853815753878099</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -3961,16 +3961,16 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>-16.931923516207</v>
+        <v>5.2377275672514596</v>
       </c>
       <c r="C44">
-        <v>96.771219936602094</v>
+        <v>86.316181523646193</v>
       </c>
       <c r="D44">
-        <v>-8.1763018883805397E-2</v>
+        <v>-0.12262279068084</v>
       </c>
       <c r="E44">
-        <v>8.3286557522071707</v>
+        <v>7.0924566502506803</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -3978,16 +3978,16 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>13.7875503302879</v>
+        <v>16.228085889245701</v>
       </c>
       <c r="C45">
-        <v>114.541229089569</v>
+        <v>113.273392492122</v>
       </c>
       <c r="D45">
-        <v>13.7875503302879</v>
+        <v>16.228085889245701</v>
       </c>
       <c r="E45">
-        <v>114.541229089569</v>
+        <v>113.273392492122</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -3995,16 +3995,16 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>-22.431295151115101</v>
+        <v>13.5796053382913</v>
       </c>
       <c r="C46">
-        <v>99.074667099206906</v>
+        <v>83.902023055044296</v>
       </c>
       <c r="D46">
-        <v>7.4381454833878202E-2</v>
+        <v>-3.88250378421141E-2</v>
       </c>
       <c r="E46">
-        <v>7.27476917028764</v>
+        <v>7.07779082913581</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -4012,16 +4012,16 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>-10.9339321001607</v>
+        <v>6.9428331868213897</v>
       </c>
       <c r="C47">
-        <v>98.553402029472295</v>
+        <v>83.025747999464301</v>
       </c>
       <c r="D47">
-        <v>4.1369658717116703E-2</v>
+        <v>6.4716568259429605E-2</v>
       </c>
       <c r="E47">
-        <v>7.6489288557822501</v>
+        <v>7.2629181083531202</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -4029,16 +4029,16 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>-19.853855260868901</v>
+        <v>6.2103281089504403</v>
       </c>
       <c r="C48">
-        <v>97.622958729129806</v>
+        <v>84.625005834080696</v>
       </c>
       <c r="D48">
-        <v>-6.8929007868546499E-2</v>
+        <v>-6.0228253343145501E-2</v>
       </c>
       <c r="E48">
-        <v>7.4881588455203802</v>
+        <v>6.8292318625129296</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4046,16 +4046,16 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>-19.711409046100801</v>
+        <v>9.0699272828671198</v>
       </c>
       <c r="C49">
-        <v>99.467916907682294</v>
+        <v>83.613976875084802</v>
       </c>
       <c r="D49">
-        <v>-0.14358012969970099</v>
+        <v>6.2070350961409802E-2</v>
       </c>
       <c r="E49">
-        <v>8.1279337283375206</v>
+        <v>7.6687770753459201</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4063,16 +4063,16 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>-19.084729813783898</v>
+        <v>8.8620382367106192</v>
       </c>
       <c r="C50">
-        <v>98.434588836287006</v>
+        <v>83.919351687935702</v>
       </c>
       <c r="D50">
-        <v>4.8937385955307999E-2</v>
+        <v>4.1632453634239099E-2</v>
       </c>
       <c r="E50">
-        <v>7.4488978979828904</v>
+        <v>7.3758417435021304</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4080,16 +4080,16 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>-19.3949735932595</v>
+        <v>8.4061789338097093</v>
       </c>
       <c r="C51">
-        <v>101.112711512328</v>
+        <v>85.020512128505999</v>
       </c>
       <c r="D51">
-        <v>-0.11693285621157599</v>
+        <v>-7.49499958356213E-2</v>
       </c>
       <c r="E51">
-        <v>7.15494037112905</v>
+        <v>6.6527631497801902</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4097,16 +4097,16 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>-18.325283864361701</v>
+        <v>7.7383268540597596</v>
       </c>
       <c r="C52">
-        <v>97.210044501225099</v>
+        <v>84.387631605532505</v>
       </c>
       <c r="D52">
-        <v>-0.55709555613941197</v>
+        <v>-0.19148575083399599</v>
       </c>
       <c r="E52">
-        <v>9.8320274870092899</v>
+        <v>8.8071898396000297</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4114,16 +4114,16 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>-20.637855995020299</v>
+        <v>8.5983857920934792</v>
       </c>
       <c r="C53">
-        <v>99.496456623990298</v>
+        <v>84.830913021837205</v>
       </c>
       <c r="D53">
-        <v>-0.14148662127575601</v>
+        <v>9.7787103508706799E-2</v>
       </c>
       <c r="E53">
-        <v>7.2228911935213098</v>
+        <v>7.0106924283953704</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4131,16 +4131,16 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>-19.0506999946919</v>
+        <v>9.4980006870852502</v>
       </c>
       <c r="C54">
-        <v>99.6832894932638</v>
+        <v>83.152455901366395</v>
       </c>
       <c r="D54">
-        <v>-3.3230783032679401E-2</v>
+        <v>-0.17279151207134999</v>
       </c>
       <c r="E54">
-        <v>7.5682032070265501</v>
+        <v>6.8779291288537001</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4148,16 +4148,16 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>-15.530030172791401</v>
+        <v>5.4720943727583098</v>
       </c>
       <c r="C55">
-        <v>101.476796027885</v>
+        <v>84.476678208048895</v>
       </c>
       <c r="D55">
-        <v>-7.3190901221677096E-2</v>
+        <v>8.4370252879750807E-2</v>
       </c>
       <c r="E55">
-        <v>7.9557750046834501</v>
+        <v>7.10121532475985</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4165,16 +4165,16 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>-23.9083726969019</v>
+        <v>9.5373024287048196</v>
       </c>
       <c r="C56">
-        <v>96.734064379037903</v>
+        <v>87.113980806857697</v>
       </c>
       <c r="D56">
-        <v>0.215403077516404</v>
+        <v>0.12732271998674</v>
       </c>
       <c r="E56">
-        <v>8.3659867354087893</v>
+        <v>7.4835268368554804</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -4182,16 +4182,16 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>14.033252344738701</v>
+        <v>21.611876570439801</v>
       </c>
       <c r="C57">
-        <v>110.92038157853101</v>
+        <v>113.394608277892</v>
       </c>
       <c r="D57">
-        <v>14.033252344738701</v>
+        <v>21.611876570439801</v>
       </c>
       <c r="E57">
-        <v>110.92038157853101</v>
+        <v>113.394608277892</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -4199,16 +4199,16 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>-26.778140959439</v>
+        <v>5.02784863138824</v>
       </c>
       <c r="C58">
-        <v>101.873964572437</v>
+        <v>84.324308433550698</v>
       </c>
       <c r="D58">
-        <v>-2.74534290043057E-2</v>
+        <v>0.477429364781007</v>
       </c>
       <c r="E58">
-        <v>9.1897741264566299</v>
+        <v>8.3393061641596606</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -4216,16 +4216,16 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>-22.495404674465298</v>
+        <v>8.7103858855391607</v>
       </c>
       <c r="C59">
-        <v>97.901813315181002</v>
+        <v>84.938488916882406</v>
       </c>
       <c r="D59">
-        <v>1.5960212607275599E-2</v>
+        <v>-1.4650697166731501E-2</v>
       </c>
       <c r="E59">
-        <v>7.7270538001747502</v>
+        <v>7.2080471661763204</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -4233,16 +4233,16 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>-8.37267523636676</v>
+        <v>6.8268979056296804</v>
       </c>
       <c r="C60">
-        <v>100.78946705880399</v>
+        <v>83.731193285324593</v>
       </c>
       <c r="D60">
-        <v>-0.28820596460929498</v>
+        <v>9.5595884192418101E-2</v>
       </c>
       <c r="E60">
-        <v>7.9307410168293497</v>
+        <v>7.1080924969268597</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -4250,16 +4250,16 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>-23.116206488230901</v>
+        <v>5.6312994227368502</v>
       </c>
       <c r="C61">
-        <v>99.689668061715196</v>
+        <v>83.221774284760798</v>
       </c>
       <c r="D61">
-        <v>-0.24453810465273601</v>
+        <v>-0.209934931215112</v>
       </c>
       <c r="E61">
-        <v>7.5163162711801901</v>
+        <v>6.9776163730675496</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -4267,16 +4267,16 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>-9.2578279084223105</v>
+        <v>6.9171130076183402</v>
       </c>
       <c r="C62">
-        <v>103.516594224153</v>
+        <v>84.203290393247201</v>
       </c>
       <c r="D62">
-        <v>-0.88119796433714004</v>
+        <v>0.21586708934842799</v>
       </c>
       <c r="E62">
-        <v>9.0504121292515904</v>
+        <v>9.0898169594069191</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -4284,16 +4284,16 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>-19.1858704085573</v>
+        <v>8.3781325405889895</v>
       </c>
       <c r="C63">
-        <v>95.759293716147297</v>
+        <v>82.057665337044995</v>
       </c>
       <c r="D63">
-        <v>-0.25666580650536203</v>
+        <v>-0.36635347540393898</v>
       </c>
       <c r="E63">
-        <v>7.4459831426556899</v>
+        <v>7.8612060546373099</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -4301,16 +4301,16 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>-22.781945871886901</v>
+        <v>9.7085486362762303</v>
       </c>
       <c r="C64">
-        <v>100.387918098631</v>
+        <v>82.665659158335401</v>
       </c>
       <c r="D64">
-        <v>-0.21671397065065801</v>
+        <v>7.2977281185312897E-3</v>
       </c>
       <c r="E64">
-        <v>7.0591479863220101</v>
+        <v>6.6863359680894696</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -4318,16 +4318,16 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>-20.176691910534501</v>
+        <v>6.2745586685752999</v>
       </c>
       <c r="C65">
-        <v>97.261723203409204</v>
+        <v>81.766857573413603</v>
       </c>
       <c r="D65">
-        <v>-0.19880524101407199</v>
+        <v>-0.186007520924898</v>
       </c>
       <c r="E65">
-        <v>6.9130388247678498</v>
+        <v>7.1985780882947497</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -4335,16 +4335,16 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>-15.2866903993181</v>
+        <v>1.9809189310256401</v>
       </c>
       <c r="C66">
-        <v>101.22072392242499</v>
+        <v>88.249724968299603</v>
       </c>
       <c r="D66">
-        <v>1.8245481247918999E-2</v>
+        <v>-7.4661853894276195E-2</v>
       </c>
       <c r="E66">
-        <v>9.5718394642682902</v>
+        <v>6.9559301645901996</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -4352,16 +4352,16 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>-15.3161898308483</v>
+        <v>4.3987242224592604</v>
       </c>
       <c r="C67">
-        <v>102.002803578315</v>
+        <v>84.647924673243196</v>
       </c>
       <c r="D67">
-        <v>-0.23813335425746199</v>
+        <v>0.34284608474920503</v>
       </c>
       <c r="E67">
-        <v>10.017230874818701</v>
+        <v>8.4890613648070801</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -4369,16 +4369,16 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>-10.708513690779499</v>
+        <v>2.1980318800568499</v>
       </c>
       <c r="C68">
-        <v>100.892933790336</v>
+        <v>87.910430936452698</v>
       </c>
       <c r="D68">
-        <v>-0.23186909464914901</v>
+        <v>-0.10204368137683401</v>
       </c>
       <c r="E68">
-        <v>7.3254622756469097</v>
+        <v>7.1810157075207801</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -4386,16 +4386,16 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>-15.5715269124284</v>
+        <v>7.1118124073843303</v>
       </c>
       <c r="C69">
-        <v>99.381532000379806</v>
+        <v>85.906475062918304</v>
       </c>
       <c r="D69">
-        <v>-0.35115536855915103</v>
+        <v>2.7118101010553501E-2</v>
       </c>
       <c r="E69">
-        <v>7.3825457342209004</v>
+        <v>7.1513240160204496</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -4403,16 +4403,16 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>-15.1547660725781</v>
+        <v>4.1439922202397996</v>
       </c>
       <c r="C70">
-        <v>103.943241126937</v>
+        <v>84.768727843478203</v>
       </c>
       <c r="D70">
-        <v>-0.24311345663230599</v>
+        <v>-0.13780831920132799</v>
       </c>
       <c r="E70">
-        <v>6.9219037288253098</v>
+        <v>6.8665736988166097</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -4420,16 +4420,16 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>-15.668777898903199</v>
+        <v>4.16248115299953</v>
       </c>
       <c r="C71">
-        <v>99.2999859174204</v>
+        <v>85.191755519779093</v>
       </c>
       <c r="D71">
-        <v>-0.413431139582769</v>
+        <v>0.13224299031846001</v>
       </c>
       <c r="E71">
-        <v>7.2340184212317098</v>
+        <v>6.9367770229960604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>